<commit_message>
[EmployeeTimesheet] Updated Timesheet template to have stronger Date and Time input validity
</commit_message>
<xml_diff>
--- a/python_source/Timesheet Calculator v2/doc/Employee Timesheet Template.xlsx
+++ b/python_source/Timesheet Calculator v2/doc/Employee Timesheet Template.xlsx
@@ -358,7 +358,7 @@
       <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
@@ -519,13 +519,13 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" error="Please input a valid date. Date Format: &#10;DD-MMM-YYYY &#10;&#10;Example:&#10;14-Jun-2021" errorTitle="Invalid Date" operator="greaterThan" prompt="Date format should be DD-MMM-YYYY e.g.&#10;14-Jun-2021&#10;03-Jan-2021" promptTitle="Date Format" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A11:A15" type="date">
+    <dataValidation allowBlank="true" error="Please input a valid time. Time format: &#10;12-hour format (HH:MM AM/PM)&#10;Military format (HH:MM)&#10;&#10;Example: 09:00 AM or 13:00" errorTitle="Time Format" operator="between" prompt="Please input a valid time. Time format: &#10;12-hour format (HH:MM AM/PM)&#10;Military format (HH:MM)&#10;&#10;Example: 09:00 AM or 13:00" promptTitle="Time Format" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B11:C15" type="time">
+      <formula1>0</formula1>
+      <formula2>0.958333333333333</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please input a valid date. Date Format: &#10;DD-MMM-YYYY &#10;&#10;Example:&#10;14-Jun-2021" errorTitle="Invalid Date" operator="greaterThan" prompt="Please input a valid date. Date Format: &#10;DD-MMM-YYYY &#10;&#10;Example:&#10;14-Jun-2021" promptTitle="Date Format" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A11:A15" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please input a valid time. Time format: &#10;12-hour format (HH:MM AM/PM)&#10;Military format (HH:MM)&#10;&#10;Example: 09:00 AM or 13:00" errorTitle="Time Format" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:C15" type="time">
-      <formula1>0</formula1>
-      <formula2>0.958333333333333</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -549,7 +549,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>